<commit_message>
Fixed GSuite credentials and email not sending
</commit_message>
<xml_diff>
--- a/Data/Input/AssociateEmails.xlsx
+++ b/Data/Input/AssociateEmails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-1\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8E1194-85B8-4367-9AD9-BF828A4A152E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6065AD2-ED5C-40FC-BC26-3660E75EF444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{3E2EB5E5-B231-441E-A577-D816897A52AE}"/>
   </bookViews>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>jewlzandtheboyz@gmail.com</t>
   </si>
   <si>
     <t>michael.bachkabakian@revature.net</t>
-  </si>
-  <si>
-    <t>wiknncsljnkv3434js@yahoo.com</t>
   </si>
   <si>
     <t>jacob.jennings@revature.net</t>
@@ -410,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E06D3300-5898-42E7-A14F-82BE77926738}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +420,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -441,17 +438,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B9587558-E4CD-4646-8D51-F1A654266199}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{2F505BBD-F97D-4C1F-9D04-5AA57235C6D5}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{3539212E-BE84-44F4-86A0-76E446BDF347}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{0C5C4FB1-346D-4702-A201-0C870C7B3B4E}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{0C5C4FB1-346D-4702-A201-0C870C7B3B4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>